<commit_message>
The generated Excel file with new formatting
</commit_message>
<xml_diff>
--- a/DesktopExcelSucks.xlsx
+++ b/DesktopExcelSucks.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Our cool Report</t>
+  </si>
   <si>
     <t>Id</t>
   </si>
@@ -46,8 +49,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF0000FF" tint="0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
@@ -74,6 +87,16 @@
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -84,62 +107,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1" style="1"/>
     <col min="2" max="2" width="9.729009628295898" customWidth="1"/>
-    <col min="3" max="3" width="9.431297302246094" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="2" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+    </row>
+    <row r="2" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>